<commit_message>
test: Add more history
</commit_message>
<xml_diff>
--- a/drlp2_hyperparameters_grid.xlsx
+++ b/drlp2_hyperparameters_grid.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ai\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ai\Documents\openAI\DeepRL_P2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F32D32-5141-4A41-8F04-0DE3730DB9C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270BDBF4-D7F2-4D24-AE5E-BCCE69B8D3CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{47E14120-D9B4-4718-BD20-5C80DAF89794}"/>
+    <workbookView xWindow="31500" yWindow="2025" windowWidth="12870" windowHeight="21000" activeTab="1" xr2:uid="{47E14120-D9B4-4718-BD20-5C80DAF89794}"/>
   </bookViews>
   <sheets>
     <sheet name="Hyper_parameter_history" sheetId="2" r:id="rId1"/>
+    <sheet name="final_runs" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>'discount_rate'</t>
   </si>
@@ -72,9 +73,6 @@
     <t>back</t>
   </si>
   <si>
-    <t>introduced 'tau'</t>
-  </si>
-  <si>
     <t>'episode_count'</t>
   </si>
   <si>
@@ -89,12 +87,33 @@
   <si>
     <t>later</t>
   </si>
+  <si>
+    <t>2*val_loss</t>
+  </si>
+  <si>
+    <t>(1/(i+1))</t>
+  </si>
+  <si>
+    <t>(1/(self.step_count))</t>
+  </si>
+  <si>
+    <t>(10/(self.step_count))</t>
+  </si>
+  <si>
+    <t>seed=0</t>
+  </si>
+  <si>
+    <t>Score after Episode #:</t>
+  </si>
+  <si>
+    <t>Episodes needed:</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -117,8 +136,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-4.9989318521683403E-2"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,8 +186,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -167,11 +222,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -185,6 +251,35 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,25 +594,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726974F5-594A-477C-A525-D44D99E123E6}">
-  <dimension ref="A2:AC22"/>
+  <dimension ref="A2:AY23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A22"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:51">
       <c r="C2" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="AE2" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AC2" s="12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:51">
+      <c r="AY3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:51">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -551,19 +653,37 @@
       <c r="U4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="Y4" t="s">
-        <v>15</v>
-      </c>
       <c r="AA4" t="s">
         <v>14</v>
       </c>
       <c r="AB4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD4" t="s">
+        <v>13</v>
+      </c>
+      <c r="AR4" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS4" t="s">
+        <v>21</v>
+      </c>
+      <c r="AT4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AV4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AW4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AX4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:51">
       <c r="A5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>1000</v>
@@ -646,8 +766,74 @@
       <c r="AC5" s="4">
         <v>1000</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AE5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AF5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AG5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AH5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AI5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AJ5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AK5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AL5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AM5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AN5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AO5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AP5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AQ5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AR5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AS5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AT5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AU5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AV5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AW5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AX5" s="4">
+        <v>1000</v>
+      </c>
+      <c r="AY5" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:51">
       <c r="A6" s="4" t="s">
         <v>0</v>
       </c>
@@ -732,76 +918,142 @@
       <c r="AC6" s="4">
         <v>0.99</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD6" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="AE6" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="AF6" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="AG6" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="AH6" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="AI6" s="16">
+        <v>0.9</v>
+      </c>
+      <c r="AJ6" s="7">
+        <v>0.95</v>
+      </c>
+      <c r="AK6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AL6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AM6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AN6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AO6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AP6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AQ6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AR6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AS6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AT6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AU6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AV6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AW6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AX6" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="AY6" s="17">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:51">
       <c r="A7" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="D7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="E7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="F7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="G7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="H7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="I7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="J7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="K7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="L7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="M7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="N7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="O7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="P7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="Q7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="R7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="S7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="T7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="U7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="V7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="W7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="X7" s="4">
-        <v>1</v>
+        <v>0.95</v>
       </c>
       <c r="Y7" s="5">
         <v>0.75</v>
@@ -818,8 +1070,74 @@
       <c r="AC7" s="6">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AE7" s="14">
+        <v>0.75</v>
+      </c>
+      <c r="AF7" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="AG7" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="AH7" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="AI7" s="6">
+        <v>0.9</v>
+      </c>
+      <c r="AJ7" s="15">
+        <v>0.95</v>
+      </c>
+      <c r="AK7" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="AL7" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="AM7" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="AN7" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="AO7" s="20">
+        <v>0.95</v>
+      </c>
+      <c r="AP7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="24">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:51">
       <c r="A8" s="4" t="s">
         <v>2</v>
       </c>
@@ -904,8 +1222,74 @@
       <c r="AC8" s="4">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AE8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AF8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AG8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AH8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AI8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AJ8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AK8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AL8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AM8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AN8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AO8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AP8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AQ8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AR8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AS8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AT8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AU8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AV8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AW8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AX8" s="4">
+        <v>15</v>
+      </c>
+      <c r="AY8" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:51">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
@@ -990,8 +1374,74 @@
       <c r="AC9" s="8">
         <v>3072</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AE9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AF9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AG9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AH9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AI9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AJ9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AK9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AL9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AM9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AN9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AO9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AP9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AQ9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AR9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AS9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AT9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AU9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AV9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AW9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AX9" s="8">
+        <v>3072</v>
+      </c>
+      <c r="AY9" s="8">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="10" spans="1:51">
       <c r="A10" s="4" t="s">
         <v>4</v>
       </c>
@@ -1076,96 +1526,228 @@
       <c r="AC10" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AE10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AF10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AG10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AH10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AI10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AJ10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AK10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AL10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AM10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AN10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AO10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AP10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AQ10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AR10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AS10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AT10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AU10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AV10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AW10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AX10" s="8">
+        <v>2</v>
+      </c>
+      <c r="AY10" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:51">
       <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="K11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="L11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="M11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="N11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="O11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="P11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Q11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="R11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="S11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="T11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="U11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="V11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="W11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="X11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Y11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="Z11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AB11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AC11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AD11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AE11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AF11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AG11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AH11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AI11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AJ11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AK11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AL11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AM11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AN11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AO11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AP11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AQ11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AR11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AS11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AT11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AU11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AV11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AW11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AX11" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="AY11" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51">
+      <c r="A12" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="G11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="H11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="I11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="J11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="K11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="L11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="M11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="N11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="O11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="P11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="Q11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="R11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="S11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="T11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="U11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="V11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="W11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="X11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="Y11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="Z11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="AA11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="AB11" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="AC11" s="4">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>18</v>
       </c>
       <c r="C12" s="4">
         <v>64</v>
@@ -1248,8 +1830,74 @@
       <c r="AC12" s="8">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AE12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AF12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AG12" s="14">
+        <v>32</v>
+      </c>
+      <c r="AH12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AI12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AJ12" s="8">
+        <v>64</v>
+      </c>
+      <c r="AK12" s="6">
+        <v>128</v>
+      </c>
+      <c r="AL12" s="5">
+        <v>32</v>
+      </c>
+      <c r="AM12" s="6">
+        <v>256</v>
+      </c>
+      <c r="AN12" s="6">
+        <v>512</v>
+      </c>
+      <c r="AO12" s="6">
+        <v>512</v>
+      </c>
+      <c r="AP12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AQ12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AR12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AS12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AT12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AU12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AV12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AW12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AX12" s="23">
+        <v>512</v>
+      </c>
+      <c r="AY12" s="23">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:51">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
@@ -1334,8 +1982,74 @@
       <c r="AC13" s="10">
         <v>2.9999999999999997E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AE13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AF13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AG13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AH13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AI13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AJ13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AK13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AL13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AM13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AN13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AO13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AP13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AQ13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AR13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AS13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AT13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AU13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AV13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AW13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AX13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="AY13" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:51">
       <c r="A14" s="4" t="s">
         <v>6</v>
       </c>
@@ -1420,8 +2134,74 @@
       <c r="AC14" s="10">
         <v>1E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AE14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AF14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AG14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AH14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AI14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AJ14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AK14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AL14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AM14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AN14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AO14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AP14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AQ14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AR14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AS14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AT14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AU14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AV14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AW14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AX14" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="AY14" s="10">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:51">
       <c r="A16" s="4">
         <v>50</v>
       </c>
@@ -1506,8 +2286,74 @@
       <c r="AC16" s="4">
         <v>1.72</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD16" s="4">
+        <v>2.13</v>
+      </c>
+      <c r="AE16" s="18">
+        <v>1.82</v>
+      </c>
+      <c r="AF16" s="18">
+        <v>1.48</v>
+      </c>
+      <c r="AG16" s="18">
+        <v>1.85</v>
+      </c>
+      <c r="AH16" s="18">
+        <v>1.5</v>
+      </c>
+      <c r="AI16" s="18">
+        <v>1.78</v>
+      </c>
+      <c r="AJ16" s="18">
+        <v>1.62</v>
+      </c>
+      <c r="AK16" s="18">
+        <v>2.06</v>
+      </c>
+      <c r="AL16" s="19">
+        <v>1.68</v>
+      </c>
+      <c r="AM16" s="19">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="AN16" s="19">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="AO16" s="19">
+        <v>2.69</v>
+      </c>
+      <c r="AP16" s="19">
+        <v>3.08</v>
+      </c>
+      <c r="AQ16" s="19">
+        <v>1.84</v>
+      </c>
+      <c r="AR16" s="19">
+        <v>2.69</v>
+      </c>
+      <c r="AS16" s="19">
+        <v>2.69</v>
+      </c>
+      <c r="AT16" s="19">
+        <v>3.59</v>
+      </c>
+      <c r="AU16" s="19">
+        <v>2.23</v>
+      </c>
+      <c r="AV16" s="19">
+        <v>2.98</v>
+      </c>
+      <c r="AW16" s="19">
+        <v>3.19</v>
+      </c>
+      <c r="AX16" s="19">
+        <v>3.91</v>
+      </c>
+      <c r="AY16" s="19">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:51">
       <c r="A17" s="4">
         <v>100</v>
       </c>
@@ -1592,8 +2438,74 @@
       <c r="AC17" s="4">
         <v>2.46</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD17" s="4">
+        <v>5.0599999999999996</v>
+      </c>
+      <c r="AE17" s="18">
+        <v>3.38</v>
+      </c>
+      <c r="AF17" s="18">
+        <v>1.96</v>
+      </c>
+      <c r="AG17" s="18">
+        <v>2.67</v>
+      </c>
+      <c r="AH17" s="18">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="AI17" s="18">
+        <v>2.25</v>
+      </c>
+      <c r="AJ17" s="18">
+        <v>2.17</v>
+      </c>
+      <c r="AK17" s="18">
+        <v>2.77</v>
+      </c>
+      <c r="AL17" s="19">
+        <v>2.58</v>
+      </c>
+      <c r="AM17" s="19">
+        <v>3.9</v>
+      </c>
+      <c r="AN17" s="19">
+        <v>5.26</v>
+      </c>
+      <c r="AO17" s="19">
+        <v>5.48</v>
+      </c>
+      <c r="AP17" s="19">
+        <v>6.5</v>
+      </c>
+      <c r="AQ17" s="19">
+        <v>3.48</v>
+      </c>
+      <c r="AR17" s="19">
+        <v>4.3899999999999997</v>
+      </c>
+      <c r="AS17" s="19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AT17" s="19">
+        <v>5.5</v>
+      </c>
+      <c r="AU17" s="19">
+        <v>3.21</v>
+      </c>
+      <c r="AV17" s="19">
+        <v>5.18</v>
+      </c>
+      <c r="AW17" s="19">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="AX17" s="19">
+        <v>10.58</v>
+      </c>
+      <c r="AY17" s="19">
+        <v>11.55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:51">
       <c r="A18" s="4">
         <v>200</v>
       </c>
@@ -1638,8 +2550,68 @@
       <c r="AC18" s="4">
         <v>5.38</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD18" s="4">
+        <v>12.67</v>
+      </c>
+      <c r="AE18" s="18">
+        <v>8.49</v>
+      </c>
+      <c r="AF18" s="18">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AG18" s="18">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AH18" s="18">
+        <v>6.78</v>
+      </c>
+      <c r="AI18" s="18">
+        <v>7.03</v>
+      </c>
+      <c r="AJ18" s="18">
+        <v>6.02</v>
+      </c>
+      <c r="AK18" s="18">
+        <v>9.67</v>
+      </c>
+      <c r="AL18" s="19">
+        <v>6.01</v>
+      </c>
+      <c r="AM18" s="19">
+        <v>11.3</v>
+      </c>
+      <c r="AN18" s="19">
+        <v>25.3</v>
+      </c>
+      <c r="AO18" s="19">
+        <v>25.64</v>
+      </c>
+      <c r="AP18" s="19">
+        <v>28.38</v>
+      </c>
+      <c r="AQ18" s="19">
+        <v>10.93</v>
+      </c>
+      <c r="AR18" s="19">
+        <v>13.94</v>
+      </c>
+      <c r="AS18" s="19">
+        <v>16.3</v>
+      </c>
+      <c r="AT18" s="19">
+        <v>23.05</v>
+      </c>
+      <c r="AU18" s="19">
+        <v>7.1</v>
+      </c>
+      <c r="AV18" s="19">
+        <v>22.3</v>
+      </c>
+      <c r="AW18" s="4"/>
+      <c r="AX18" s="4"/>
+      <c r="AY18" s="4"/>
+    </row>
+    <row r="19" spans="1:51">
       <c r="A19" s="4">
         <v>300</v>
       </c>
@@ -1680,8 +2652,54 @@
       <c r="AC19" s="4">
         <v>7.06</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD19" s="4"/>
+      <c r="AE19" s="18">
+        <v>14.35</v>
+      </c>
+      <c r="AF19" s="18">
+        <v>5.88</v>
+      </c>
+      <c r="AG19" s="18">
+        <v>8.85</v>
+      </c>
+      <c r="AH19" s="18">
+        <v>10.47</v>
+      </c>
+      <c r="AI19" s="18">
+        <v>10.56</v>
+      </c>
+      <c r="AJ19" s="18">
+        <v>14.91</v>
+      </c>
+      <c r="AK19" s="18">
+        <v>15.29</v>
+      </c>
+      <c r="AL19" s="19">
+        <v>10.64</v>
+      </c>
+      <c r="AM19" s="4"/>
+      <c r="AN19" s="4"/>
+      <c r="AO19" s="4"/>
+      <c r="AP19" s="4"/>
+      <c r="AQ19" s="4">
+        <v>16.3</v>
+      </c>
+      <c r="AR19" s="4">
+        <v>25.21</v>
+      </c>
+      <c r="AS19" s="4">
+        <v>27.86</v>
+      </c>
+      <c r="AT19" s="4"/>
+      <c r="AU19" s="21">
+        <v>14.82</v>
+      </c>
+      <c r="AV19" s="4"/>
+      <c r="AW19" s="4"/>
+      <c r="AX19" s="4"/>
+      <c r="AY19" s="4"/>
+    </row>
+    <row r="20" spans="1:51">
       <c r="A20" s="4">
         <v>500</v>
       </c>
@@ -1726,8 +2744,46 @@
       <c r="AC20" s="4">
         <v>15.37</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD20" s="4"/>
+      <c r="AE20" s="18">
+        <v>29.95</v>
+      </c>
+      <c r="AF20" s="18">
+        <v>8.6300000000000008</v>
+      </c>
+      <c r="AG20" s="18">
+        <v>19.53</v>
+      </c>
+      <c r="AH20" s="18">
+        <v>18.63</v>
+      </c>
+      <c r="AI20" s="18">
+        <v>17.920000000000002</v>
+      </c>
+      <c r="AJ20" s="4"/>
+      <c r="AK20" s="18">
+        <v>23.18</v>
+      </c>
+      <c r="AL20" s="19">
+        <v>18.11</v>
+      </c>
+      <c r="AM20" s="4"/>
+      <c r="AN20" s="4"/>
+      <c r="AO20" s="4"/>
+      <c r="AP20" s="4"/>
+      <c r="AQ20" s="4">
+        <v>24.99</v>
+      </c>
+      <c r="AR20" s="4"/>
+      <c r="AS20" s="4"/>
+      <c r="AT20" s="4"/>
+      <c r="AU20" s="4"/>
+      <c r="AV20" s="4"/>
+      <c r="AW20" s="4"/>
+      <c r="AX20" s="4"/>
+      <c r="AY20" s="4"/>
+    </row>
+    <row r="21" spans="1:51">
       <c r="A21" s="4">
         <v>750</v>
       </c>
@@ -1766,8 +2822,38 @@
       <c r="AC21" s="4">
         <v>21.42</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="AD21" s="4"/>
+      <c r="AE21" s="4"/>
+      <c r="AF21" s="18">
+        <v>11.23</v>
+      </c>
+      <c r="AG21" s="18">
+        <v>24.27</v>
+      </c>
+      <c r="AH21" s="4"/>
+      <c r="AI21" s="18">
+        <v>23.03</v>
+      </c>
+      <c r="AJ21" s="4"/>
+      <c r="AK21" s="4"/>
+      <c r="AL21" s="4">
+        <v>22.06</v>
+      </c>
+      <c r="AM21" s="4"/>
+      <c r="AN21" s="4"/>
+      <c r="AO21" s="4"/>
+      <c r="AP21" s="4"/>
+      <c r="AQ21" s="4"/>
+      <c r="AR21" s="4"/>
+      <c r="AS21" s="4"/>
+      <c r="AT21" s="4"/>
+      <c r="AU21" s="4"/>
+      <c r="AV21" s="4"/>
+      <c r="AW21" s="4"/>
+      <c r="AX21" s="4"/>
+      <c r="AY21" s="4"/>
+    </row>
+    <row r="22" spans="1:51">
       <c r="A22" s="4">
         <v>1000</v>
       </c>
@@ -1812,9 +2898,105 @@
       <c r="AC22" s="4">
         <v>29.44</v>
       </c>
+      <c r="AD22" s="4"/>
+      <c r="AE22" s="4"/>
+      <c r="AF22" s="18">
+        <v>14.28</v>
+      </c>
+      <c r="AG22" s="4"/>
+      <c r="AH22" s="4"/>
+      <c r="AI22" s="18">
+        <v>28.48</v>
+      </c>
+      <c r="AJ22" s="4"/>
+      <c r="AK22" s="4"/>
+      <c r="AL22" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="AM22" s="4"/>
+      <c r="AN22" s="4"/>
+      <c r="AO22" s="4"/>
+      <c r="AP22" s="4"/>
+      <c r="AQ22" s="4"/>
+      <c r="AR22" s="4"/>
+      <c r="AS22" s="4"/>
+      <c r="AT22" s="4"/>
+      <c r="AU22" s="4"/>
+      <c r="AV22" s="4"/>
+      <c r="AW22" s="4"/>
+      <c r="AX22" s="4"/>
+      <c r="AY22" s="4"/>
+    </row>
+    <row r="23" spans="1:51">
+      <c r="AC23">
+        <v>1001</v>
+      </c>
+      <c r="AD23">
+        <v>285</v>
+      </c>
+      <c r="AE23" s="13">
+        <v>501</v>
+      </c>
+      <c r="AG23" s="13">
+        <v>802</v>
+      </c>
+      <c r="AH23" s="13">
+        <v>623</v>
+      </c>
+      <c r="AI23" s="13">
+        <v>1103</v>
+      </c>
+      <c r="AJ23" s="13">
+        <v>399</v>
+      </c>
+      <c r="AK23" s="13">
+        <v>660</v>
+      </c>
+      <c r="AL23" s="13">
+        <v>1385</v>
+      </c>
+      <c r="AM23" s="13">
+        <v>291</v>
+      </c>
+      <c r="AN23" s="13">
+        <v>230</v>
+      </c>
+      <c r="AO23" s="13">
+        <v>234</v>
+      </c>
+      <c r="AP23" s="13">
+        <v>211</v>
+      </c>
+      <c r="AQ23" s="13">
+        <v>686</v>
+      </c>
+      <c r="AR23" s="13">
+        <v>398</v>
+      </c>
+      <c r="AS23" s="13">
+        <v>319</v>
+      </c>
+      <c r="AT23" s="13">
+        <v>229</v>
+      </c>
+      <c r="AU23" s="13">
+        <v>499</v>
+      </c>
+      <c r="AV23" s="13">
+        <v>245</v>
+      </c>
+      <c r="AW23" s="13">
+        <v>171</v>
+      </c>
+      <c r="AX23" s="13">
+        <v>164</v>
+      </c>
+      <c r="AY23" s="13">
+        <v>191</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C16:AC16">
+  <conditionalFormatting sqref="C16:AZ16">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -1824,7 +3006,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C17:AC17">
+  <conditionalFormatting sqref="C17:AZ17">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -1834,7 +3016,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C18:AC18">
+  <conditionalFormatting sqref="C18:AZ18">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
@@ -1844,7 +3026,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C19:AC19">
+  <conditionalFormatting sqref="C19:AZ19">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1854,7 +3036,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R20:AC20">
+  <conditionalFormatting sqref="R20:AZ20">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1864,7 +3046,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R21:AC21">
+  <conditionalFormatting sqref="R21:AZ21">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -1874,7 +3056,534 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="R22:AC22">
+  <conditionalFormatting sqref="R22:AZ22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DEC3ECF-12D6-4592-A12B-A5AB4423DE63}">
+  <dimension ref="B3:I22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:9">
+      <c r="B3" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" hidden="1">
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="D4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="G4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="I4" s="4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="E5" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="F5" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="G5" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="H5" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="I5" s="17">
+        <v>0.95</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" hidden="1">
+      <c r="B6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24">
+        <v>0</v>
+      </c>
+      <c r="D6" s="24">
+        <v>0</v>
+      </c>
+      <c r="E6" s="24">
+        <v>0</v>
+      </c>
+      <c r="F6" s="24">
+        <v>0</v>
+      </c>
+      <c r="G6" s="24">
+        <v>0</v>
+      </c>
+      <c r="H6" s="24">
+        <v>0</v>
+      </c>
+      <c r="I6" s="24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="4">
+        <v>15</v>
+      </c>
+      <c r="D7" s="4">
+        <v>15</v>
+      </c>
+      <c r="E7" s="4">
+        <v>15</v>
+      </c>
+      <c r="F7" s="4">
+        <v>15</v>
+      </c>
+      <c r="G7" s="4">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4">
+        <v>15</v>
+      </c>
+      <c r="I7" s="4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="8">
+        <v>3072</v>
+      </c>
+      <c r="D8" s="8">
+        <v>3072</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3072</v>
+      </c>
+      <c r="F8" s="8">
+        <v>3072</v>
+      </c>
+      <c r="G8" s="8">
+        <v>3072</v>
+      </c>
+      <c r="H8" s="8">
+        <v>3072</v>
+      </c>
+      <c r="I8" s="8">
+        <v>3072</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>2</v>
+      </c>
+      <c r="E9" s="8">
+        <v>2</v>
+      </c>
+      <c r="F9" s="8">
+        <v>2</v>
+      </c>
+      <c r="G9" s="8">
+        <v>2</v>
+      </c>
+      <c r="H9" s="8">
+        <v>2</v>
+      </c>
+      <c r="I9" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="H10" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="I10" s="4">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="23">
+        <v>512</v>
+      </c>
+      <c r="D11" s="23">
+        <v>512</v>
+      </c>
+      <c r="E11" s="23">
+        <v>512</v>
+      </c>
+      <c r="F11" s="23">
+        <v>512</v>
+      </c>
+      <c r="G11" s="23">
+        <v>512</v>
+      </c>
+      <c r="H11" s="23">
+        <v>512</v>
+      </c>
+      <c r="I11" s="23">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="D12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="F12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="H12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="I12" s="10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="D13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="F13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="G13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="H13" s="10">
+        <v>1E-4</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="22">
+        <v>50</v>
+      </c>
+      <c r="C15" s="19">
+        <v>2.69</v>
+      </c>
+      <c r="D15" s="19">
+        <v>3.59</v>
+      </c>
+      <c r="E15" s="19">
+        <v>2.23</v>
+      </c>
+      <c r="F15" s="19">
+        <v>2.98</v>
+      </c>
+      <c r="G15" s="19">
+        <v>3.19</v>
+      </c>
+      <c r="H15" s="19">
+        <v>3.91</v>
+      </c>
+      <c r="I15" s="19">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="22">
+        <v>100</v>
+      </c>
+      <c r="C16" s="19">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D16" s="19">
+        <v>5.5</v>
+      </c>
+      <c r="E16" s="19">
+        <v>3.21</v>
+      </c>
+      <c r="F16" s="19">
+        <v>5.18</v>
+      </c>
+      <c r="G16" s="19">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="H16" s="19">
+        <v>10.58</v>
+      </c>
+      <c r="I16" s="19">
+        <v>11.55</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="22">
+        <v>200</v>
+      </c>
+      <c r="C17" s="19">
+        <v>16.3</v>
+      </c>
+      <c r="D17" s="19">
+        <v>23.05</v>
+      </c>
+      <c r="E17" s="19">
+        <v>7.1</v>
+      </c>
+      <c r="F17" s="19">
+        <v>22.3</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="2:9">
+      <c r="B18" s="22">
+        <v>300</v>
+      </c>
+      <c r="C18" s="4">
+        <v>27.86</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="21">
+        <v>14.82</v>
+      </c>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="2:9">
+      <c r="B19" s="22">
+        <v>500</v>
+      </c>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="2:9">
+      <c r="B20" s="22">
+        <v>750</v>
+      </c>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="2:9">
+      <c r="B21" s="22">
+        <v>1000</v>
+      </c>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="2:9">
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="28">
+        <v>319</v>
+      </c>
+      <c r="D22" s="28">
+        <v>229</v>
+      </c>
+      <c r="E22" s="28">
+        <v>499</v>
+      </c>
+      <c r="F22" s="28">
+        <v>245</v>
+      </c>
+      <c r="G22" s="28">
+        <v>171</v>
+      </c>
+      <c r="H22" s="28">
+        <v>164</v>
+      </c>
+      <c r="I22" s="28">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C15:I15">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C16:I16">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C17:I17">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18:I18">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19:I19">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C20:I20">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21:I21">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>